<commit_message>
Update OED transform spec. - add descriptions to existing FM level IDs
</commit_message>
<xml_diff>
--- a/oed_transform_spec.xlsx
+++ b/oed_transform_spec.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="454">
   <si>
     <t>Purpose</t>
   </si>
@@ -977,9 +977,21 @@
     <t>site</t>
   </si>
   <si>
+    <t>1 (Coverage)</t>
+  </si>
+  <si>
+    <t>2 (Combined)</t>
+  </si>
+  <si>
+    <t>3 (Site)</t>
+  </si>
+  <si>
     <t>cond</t>
   </si>
   <si>
+    <t>4 (Sublimit)</t>
+  </si>
+  <si>
     <t>policy</t>
   </si>
   <si>
@@ -992,7 +1004,13 @@
     <t xml:space="preserve">    9 </t>
   </si>
   <si>
+    <t>5 (Account)</t>
+  </si>
+  <si>
     <t xml:space="preserve">    10 </t>
+  </si>
+  <si>
+    <t>6 (Layer/Policy)</t>
   </si>
   <si>
     <t>account</t>
@@ -11079,7 +11097,7 @@
     <col min="1" max="1" width="24.8516" style="12" customWidth="1"/>
     <col min="2" max="2" width="12.5" style="12" customWidth="1"/>
     <col min="3" max="3" width="23.5" style="12" customWidth="1"/>
-    <col min="4" max="4" width="8.85156" style="12" customWidth="1"/>
+    <col min="4" max="4" width="17.1953" style="12" customWidth="1"/>
     <col min="5" max="5" width="8.85156" style="12" customWidth="1"/>
     <col min="6" max="6" width="8.85156" style="12" customWidth="1"/>
     <col min="7" max="7" width="22.1719" style="12" customWidth="1"/>
@@ -12881,8 +12899,8 @@
       <c r="C47" t="s" s="20">
         <v>289</v>
       </c>
-      <c r="D47" s="18">
-        <v>1</v>
+      <c r="D47" t="s" s="20">
+        <v>320</v>
       </c>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
@@ -12925,8 +12943,8 @@
       <c r="C48" t="s" s="4">
         <v>294</v>
       </c>
-      <c r="D48" s="10">
-        <v>2</v>
+      <c r="D48" t="s" s="4">
+        <v>321</v>
       </c>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
@@ -12965,8 +12983,8 @@
       <c r="C49" t="s" s="4">
         <v>295</v>
       </c>
-      <c r="D49" s="10">
-        <v>3</v>
+      <c r="D49" t="s" s="4">
+        <v>322</v>
       </c>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
@@ -12999,7 +13017,7 @@
     </row>
     <row r="50" ht="15" customHeight="1">
       <c r="A50" t="s" s="4">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="B50" t="s" s="9">
         <v>53</v>
@@ -13087,8 +13105,8 @@
       <c r="C52" t="s" s="4">
         <v>298</v>
       </c>
-      <c r="D52" s="10">
-        <v>4</v>
+      <c r="D52" t="s" s="4">
+        <v>324</v>
       </c>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
@@ -13121,10 +13139,10 @@
     </row>
     <row r="53" ht="15" customHeight="1">
       <c r="A53" t="s" s="4">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="B53" t="s" s="9">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="C53" t="s" s="4">
         <v>299</v>
@@ -13166,7 +13184,7 @@
     <row r="54" ht="15" customHeight="1">
       <c r="A54" s="3"/>
       <c r="B54" t="s" s="9">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="C54" t="s" s="4">
         <v>300</v>
@@ -13204,13 +13222,13 @@
     <row r="55" ht="15" customHeight="1">
       <c r="A55" s="3"/>
       <c r="B55" t="s" s="9">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="C55" t="s" s="4">
         <v>301</v>
       </c>
-      <c r="D55" s="10">
-        <v>5</v>
+      <c r="D55" t="s" s="4">
+        <v>329</v>
       </c>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
@@ -13244,13 +13262,13 @@
     <row r="56" ht="15" customHeight="1">
       <c r="A56" s="3"/>
       <c r="B56" t="s" s="9">
-        <v>325</v>
+        <v>330</v>
       </c>
       <c r="C56" t="s" s="4">
         <v>302</v>
       </c>
-      <c r="D56" s="10">
-        <v>6</v>
+      <c r="D56" t="s" s="4">
+        <v>331</v>
       </c>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
@@ -13274,10 +13292,10 @@
     </row>
     <row r="57" ht="15" customHeight="1">
       <c r="A57" t="s" s="4">
-        <v>326</v>
+        <v>332</v>
       </c>
       <c r="B57" t="s" s="9">
-        <v>327</v>
+        <v>333</v>
       </c>
       <c r="C57" t="s" s="4">
         <v>303</v>
@@ -13306,7 +13324,7 @@
     <row r="58" ht="15" customHeight="1">
       <c r="A58" s="3"/>
       <c r="B58" t="s" s="9">
-        <v>328</v>
+        <v>334</v>
       </c>
       <c r="C58" t="s" s="4">
         <v>304</v>
@@ -13335,7 +13353,7 @@
     <row r="59" ht="15" customHeight="1">
       <c r="A59" s="3"/>
       <c r="B59" t="s" s="9">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="C59" t="s" s="4">
         <v>305</v>
@@ -13413,10 +13431,10 @@
     </row>
     <row r="62" ht="15" customHeight="1">
       <c r="A62" t="s" s="17">
-        <v>330</v>
+        <v>336</v>
       </c>
       <c r="B62" t="s" s="17">
-        <v>331</v>
+        <v>337</v>
       </c>
       <c r="C62" s="23"/>
       <c r="D62" s="3"/>
@@ -13445,7 +13463,7 @@
         <v>1</v>
       </c>
       <c r="B63" t="s" s="20">
-        <v>332</v>
+        <v>338</v>
       </c>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
@@ -13474,7 +13492,7 @@
         <v>2</v>
       </c>
       <c r="B64" t="s" s="4">
-        <v>333</v>
+        <v>339</v>
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
@@ -13512,7 +13530,7 @@
         <v>3</v>
       </c>
       <c r="B65" t="s" s="4">
-        <v>334</v>
+        <v>340</v>
       </c>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
@@ -13550,7 +13568,7 @@
         <v>4</v>
       </c>
       <c r="B66" t="s" s="4">
-        <v>335</v>
+        <v>341</v>
       </c>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
@@ -13592,7 +13610,7 @@
         <v>5</v>
       </c>
       <c r="B67" t="s" s="4">
-        <v>336</v>
+        <v>342</v>
       </c>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
@@ -13634,7 +13652,7 @@
         <v>6</v>
       </c>
       <c r="B68" t="s" s="4">
-        <v>337</v>
+        <v>343</v>
       </c>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
@@ -13707,7 +13725,7 @@
     </row>
     <row r="70" ht="15" customHeight="1">
       <c r="A70" t="s" s="6">
-        <v>338</v>
+        <v>344</v>
       </c>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
@@ -13743,13 +13761,13 @@
     </row>
     <row r="71" ht="15" customHeight="1">
       <c r="A71" t="s" s="24">
-        <v>339</v>
+        <v>345</v>
       </c>
       <c r="B71" t="s" s="6">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="C71" t="s" s="25">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="D71" s="3"/>
       <c r="E71" s="3"/>
@@ -13791,10 +13809,10 @@
         <v>1</v>
       </c>
       <c r="B72" t="s" s="4">
-        <v>342</v>
+        <v>348</v>
       </c>
       <c r="C72" t="s" s="27">
-        <v>343</v>
+        <v>349</v>
       </c>
       <c r="D72" s="3"/>
       <c r="E72" s="3"/>
@@ -13836,10 +13854,10 @@
         <v>1</v>
       </c>
       <c r="B73" t="s" s="4">
-        <v>344</v>
+        <v>350</v>
       </c>
       <c r="C73" t="s" s="27">
-        <v>345</v>
+        <v>351</v>
       </c>
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
@@ -13881,10 +13899,10 @@
         <v>1</v>
       </c>
       <c r="B74" t="s" s="4">
-        <v>346</v>
+        <v>352</v>
       </c>
       <c r="C74" t="s" s="27">
-        <v>347</v>
+        <v>353</v>
       </c>
       <c r="D74" s="3"/>
       <c r="E74" s="3"/>
@@ -13922,10 +13940,10 @@
         <v>1</v>
       </c>
       <c r="B75" t="s" s="4">
-        <v>348</v>
+        <v>354</v>
       </c>
       <c r="C75" t="s" s="27">
-        <v>349</v>
+        <v>355</v>
       </c>
       <c r="D75" s="3"/>
       <c r="E75" s="3"/>
@@ -13963,10 +13981,10 @@
         <v>1</v>
       </c>
       <c r="B76" t="s" s="4">
-        <v>350</v>
+        <v>356</v>
       </c>
       <c r="C76" t="s" s="27">
-        <v>351</v>
+        <v>357</v>
       </c>
       <c r="D76" s="3"/>
       <c r="E76" s="3"/>
@@ -14008,10 +14026,10 @@
         <v>1</v>
       </c>
       <c r="B77" t="s" s="4">
-        <v>352</v>
+        <v>358</v>
       </c>
       <c r="C77" t="s" s="27">
-        <v>353</v>
+        <v>359</v>
       </c>
       <c r="D77" s="3"/>
       <c r="E77" s="3"/>
@@ -14053,10 +14071,10 @@
         <v>1</v>
       </c>
       <c r="B78" t="s" s="4">
-        <v>354</v>
+        <v>360</v>
       </c>
       <c r="C78" t="s" s="27">
-        <v>355</v>
+        <v>361</v>
       </c>
       <c r="D78" s="3"/>
       <c r="E78" s="3"/>
@@ -14098,10 +14116,10 @@
         <v>1</v>
       </c>
       <c r="B79" t="s" s="4">
-        <v>356</v>
+        <v>362</v>
       </c>
       <c r="C79" t="s" s="27">
-        <v>357</v>
+        <v>363</v>
       </c>
       <c r="D79" s="3"/>
       <c r="E79" s="3"/>
@@ -14139,10 +14157,10 @@
         <v>1</v>
       </c>
       <c r="B80" t="s" s="4">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="C80" t="s" s="27">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="D80" s="3"/>
       <c r="E80" s="3"/>
@@ -14180,10 +14198,10 @@
         <v>1</v>
       </c>
       <c r="B81" t="s" s="4">
-        <v>360</v>
+        <v>366</v>
       </c>
       <c r="C81" t="s" s="27">
-        <v>361</v>
+        <v>367</v>
       </c>
       <c r="D81" s="3"/>
       <c r="E81" s="3"/>
@@ -14225,10 +14243,10 @@
         <v>1</v>
       </c>
       <c r="B82" t="s" s="4">
-        <v>362</v>
+        <v>368</v>
       </c>
       <c r="C82" t="s" s="27">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="D82" s="3"/>
       <c r="E82" s="3"/>
@@ -14270,10 +14288,10 @@
         <v>1</v>
       </c>
       <c r="B83" t="s" s="4">
-        <v>364</v>
+        <v>370</v>
       </c>
       <c r="C83" t="s" s="27">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="D83" s="3"/>
       <c r="E83" s="3"/>
@@ -14315,10 +14333,10 @@
         <v>1</v>
       </c>
       <c r="B84" t="s" s="4">
-        <v>366</v>
+        <v>372</v>
       </c>
       <c r="C84" t="s" s="27">
-        <v>367</v>
+        <v>373</v>
       </c>
       <c r="D84" s="3"/>
       <c r="E84" s="3"/>
@@ -14356,10 +14374,10 @@
         <v>1</v>
       </c>
       <c r="B85" t="s" s="4">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="C85" t="s" s="27">
-        <v>369</v>
+        <v>375</v>
       </c>
       <c r="D85" s="3"/>
       <c r="E85" s="3"/>
@@ -14397,10 +14415,10 @@
         <v>1</v>
       </c>
       <c r="B86" t="s" s="4">
-        <v>370</v>
+        <v>376</v>
       </c>
       <c r="C86" t="s" s="27">
-        <v>371</v>
+        <v>377</v>
       </c>
       <c r="D86" s="3"/>
       <c r="E86" s="3"/>
@@ -14442,10 +14460,10 @@
         <v>1</v>
       </c>
       <c r="B87" t="s" s="4">
-        <v>372</v>
+        <v>378</v>
       </c>
       <c r="C87" t="s" s="27">
-        <v>373</v>
+        <v>379</v>
       </c>
       <c r="D87" s="3"/>
       <c r="E87" s="3"/>
@@ -14487,10 +14505,10 @@
         <v>1</v>
       </c>
       <c r="B88" t="s" s="4">
-        <v>374</v>
+        <v>380</v>
       </c>
       <c r="C88" t="s" s="27">
-        <v>375</v>
+        <v>381</v>
       </c>
       <c r="D88" s="3"/>
       <c r="E88" s="3"/>
@@ -14532,10 +14550,10 @@
         <v>1</v>
       </c>
       <c r="B89" t="s" s="4">
-        <v>376</v>
+        <v>382</v>
       </c>
       <c r="C89" t="s" s="27">
-        <v>377</v>
+        <v>383</v>
       </c>
       <c r="D89" s="3"/>
       <c r="E89" s="3"/>
@@ -14573,10 +14591,10 @@
         <v>1</v>
       </c>
       <c r="B90" t="s" s="4">
-        <v>378</v>
+        <v>384</v>
       </c>
       <c r="C90" t="s" s="27">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="D90" s="3"/>
       <c r="E90" s="3"/>
@@ -14614,10 +14632,10 @@
         <v>1</v>
       </c>
       <c r="B91" t="s" s="4">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="C91" t="s" s="27">
-        <v>381</v>
+        <v>387</v>
       </c>
       <c r="D91" s="3"/>
       <c r="E91" s="3"/>
@@ -14661,10 +14679,10 @@
         <v>1</v>
       </c>
       <c r="B92" t="s" s="4">
-        <v>382</v>
+        <v>388</v>
       </c>
       <c r="C92" t="s" s="27">
-        <v>383</v>
+        <v>389</v>
       </c>
       <c r="D92" s="3"/>
       <c r="E92" s="3"/>
@@ -14706,10 +14724,10 @@
         <v>1</v>
       </c>
       <c r="B93" t="s" s="4">
-        <v>384</v>
+        <v>390</v>
       </c>
       <c r="C93" t="s" s="27">
-        <v>385</v>
+        <v>391</v>
       </c>
       <c r="D93" s="3"/>
       <c r="E93" s="3"/>
@@ -14751,10 +14769,10 @@
         <v>1</v>
       </c>
       <c r="B94" t="s" s="4">
-        <v>386</v>
+        <v>392</v>
       </c>
       <c r="C94" t="s" s="27">
-        <v>387</v>
+        <v>393</v>
       </c>
       <c r="D94" s="3"/>
       <c r="E94" s="3"/>
@@ -14792,10 +14810,10 @@
         <v>1</v>
       </c>
       <c r="B95" t="s" s="4">
-        <v>388</v>
+        <v>394</v>
       </c>
       <c r="C95" t="s" s="27">
-        <v>389</v>
+        <v>395</v>
       </c>
       <c r="D95" s="3"/>
       <c r="E95" s="3"/>
@@ -14899,7 +14917,7 @@
     </row>
     <row r="98" ht="15" customHeight="1">
       <c r="A98" t="s" s="6">
-        <v>390</v>
+        <v>396</v>
       </c>
       <c r="B98" s="3"/>
       <c r="C98" s="29"/>
@@ -14935,13 +14953,13 @@
     </row>
     <row r="99" ht="15" customHeight="1">
       <c r="A99" t="s" s="24">
-        <v>339</v>
+        <v>345</v>
       </c>
       <c r="B99" t="s" s="6">
-        <v>391</v>
+        <v>397</v>
       </c>
       <c r="C99" t="s" s="25">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="D99" s="3"/>
       <c r="E99" s="3"/>
@@ -14981,10 +14999,10 @@
         <v>6</v>
       </c>
       <c r="B100" t="s" s="4">
-        <v>392</v>
+        <v>398</v>
       </c>
       <c r="C100" t="s" s="27">
-        <v>393</v>
+        <v>399</v>
       </c>
       <c r="D100" s="3"/>
       <c r="E100" s="3"/>
@@ -15022,10 +15040,10 @@
         <v>3</v>
       </c>
       <c r="B101" t="s" s="4">
-        <v>394</v>
+        <v>400</v>
       </c>
       <c r="C101" t="s" s="27">
-        <v>395</v>
+        <v>401</v>
       </c>
       <c r="D101" s="3"/>
       <c r="E101" s="3"/>
@@ -15063,10 +15081,10 @@
         <v>2</v>
       </c>
       <c r="B102" t="s" s="4">
-        <v>396</v>
+        <v>402</v>
       </c>
       <c r="C102" t="s" s="27">
-        <v>397</v>
+        <v>403</v>
       </c>
       <c r="D102" s="3"/>
       <c r="E102" s="3"/>
@@ -15106,10 +15124,10 @@
         <v>2</v>
       </c>
       <c r="B103" t="s" s="4">
-        <v>398</v>
+        <v>404</v>
       </c>
       <c r="C103" t="s" s="27">
-        <v>399</v>
+        <v>405</v>
       </c>
       <c r="D103" s="3"/>
       <c r="E103" s="3"/>
@@ -15147,10 +15165,10 @@
         <v>4</v>
       </c>
       <c r="B104" t="s" s="4">
-        <v>400</v>
+        <v>406</v>
       </c>
       <c r="C104" t="s" s="27">
-        <v>401</v>
+        <v>407</v>
       </c>
       <c r="D104" s="3"/>
       <c r="E104" s="3"/>
@@ -15188,10 +15206,10 @@
         <v>4</v>
       </c>
       <c r="B105" t="s" s="4">
-        <v>402</v>
+        <v>408</v>
       </c>
       <c r="C105" t="s" s="27">
-        <v>403</v>
+        <v>409</v>
       </c>
       <c r="D105" s="3"/>
       <c r="E105" s="3"/>
@@ -15231,10 +15249,10 @@
         <v>8</v>
       </c>
       <c r="B106" t="s" s="4">
-        <v>404</v>
+        <v>410</v>
       </c>
       <c r="C106" t="s" s="27">
-        <v>405</v>
+        <v>411</v>
       </c>
       <c r="D106" s="3"/>
       <c r="E106" s="3"/>
@@ -15272,10 +15290,10 @@
         <v>2</v>
       </c>
       <c r="B107" t="s" s="4">
-        <v>406</v>
+        <v>412</v>
       </c>
       <c r="C107" t="s" s="27">
-        <v>407</v>
+        <v>413</v>
       </c>
       <c r="D107" s="3"/>
       <c r="E107" s="3"/>
@@ -15313,10 +15331,10 @@
         <v>2</v>
       </c>
       <c r="B108" t="s" s="4">
-        <v>408</v>
+        <v>414</v>
       </c>
       <c r="C108" t="s" s="27">
-        <v>409</v>
+        <v>415</v>
       </c>
       <c r="D108" s="3"/>
       <c r="E108" s="3"/>
@@ -15356,10 +15374,10 @@
         <v>24</v>
       </c>
       <c r="B109" t="s" s="4">
-        <v>410</v>
+        <v>416</v>
       </c>
       <c r="C109" t="s" s="27">
-        <v>411</v>
+        <v>417</v>
       </c>
       <c r="D109" s="3"/>
       <c r="E109" s="3"/>
@@ -15465,7 +15483,7 @@
     </row>
     <row r="112" ht="15" customHeight="1">
       <c r="A112" t="s" s="6">
-        <v>412</v>
+        <v>418</v>
       </c>
       <c r="B112" s="3"/>
       <c r="C112" s="29"/>
@@ -15526,13 +15544,13 @@
     </row>
     <row r="114" ht="15" customHeight="1">
       <c r="A114" t="s" s="24">
-        <v>339</v>
+        <v>345</v>
       </c>
       <c r="B114" t="s" s="6">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="C114" t="s" s="25">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="D114" s="3"/>
       <c r="E114" s="3"/>
@@ -15570,10 +15588,10 @@
         <v>4</v>
       </c>
       <c r="B115" t="s" s="4">
-        <v>413</v>
+        <v>419</v>
       </c>
       <c r="C115" t="s" s="27">
-        <v>414</v>
+        <v>420</v>
       </c>
       <c r="D115" s="3"/>
       <c r="E115" s="3"/>
@@ -15615,10 +15633,10 @@
         <v>3</v>
       </c>
       <c r="B116" t="s" s="4">
-        <v>415</v>
+        <v>421</v>
       </c>
       <c r="C116" t="s" s="27">
-        <v>416</v>
+        <v>422</v>
       </c>
       <c r="D116" s="3"/>
       <c r="E116" s="3"/>
@@ -15660,10 +15678,10 @@
         <v>3</v>
       </c>
       <c r="B117" t="s" s="4">
-        <v>417</v>
+        <v>423</v>
       </c>
       <c r="C117" t="s" s="27">
-        <v>418</v>
+        <v>424</v>
       </c>
       <c r="D117" s="3"/>
       <c r="E117" s="3"/>
@@ -15705,10 +15723,10 @@
         <v>24</v>
       </c>
       <c r="B118" t="s" s="4">
-        <v>419</v>
+        <v>425</v>
       </c>
       <c r="C118" t="s" s="27">
-        <v>411</v>
+        <v>417</v>
       </c>
       <c r="D118" s="3"/>
       <c r="E118" s="3"/>
@@ -19476,7 +19494,7 @@
     <row r="1" ht="15" customHeight="1">
       <c r="A1" s="3"/>
       <c r="B1" t="s" s="6">
-        <v>420</v>
+        <v>426</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -19488,7 +19506,7 @@
     <row r="2" ht="15" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" t="s" s="4">
-        <v>421</v>
+        <v>427</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -19510,7 +19528,7 @@
     <row r="4" ht="15" customHeight="1">
       <c r="A4" s="3"/>
       <c r="B4" t="s" s="6">
-        <v>422</v>
+        <v>428</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -19552,7 +19570,7 @@
         <v>311</v>
       </c>
       <c r="H6" t="s" s="32">
-        <v>423</v>
+        <v>429</v>
       </c>
     </row>
     <row r="7" ht="15" customHeight="1">
@@ -19582,7 +19600,7 @@
     <row r="8" ht="15" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" t="s" s="4">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="C8" s="10">
         <v>0</v>
@@ -19594,7 +19612,7 @@
         <v>0</v>
       </c>
       <c r="F8" t="s" s="4">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="G8" s="33">
         <v>0</v>
@@ -19606,7 +19624,7 @@
     <row r="9" ht="15" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" t="s" s="4">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="C9" s="10">
         <v>2</v>
@@ -19618,7 +19636,7 @@
         <v>0</v>
       </c>
       <c r="F9" t="s" s="4">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="G9" s="33">
         <v>0</v>
@@ -19630,7 +19648,7 @@
     <row r="10" ht="15" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" t="s" s="4">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="C10" s="10">
         <v>1</v>
@@ -19642,7 +19660,7 @@
         <v>0</v>
       </c>
       <c r="F10" t="s" s="4">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="G10" s="33">
         <v>1</v>
@@ -19654,7 +19672,7 @@
     <row r="11" ht="15" customHeight="1">
       <c r="A11" s="3"/>
       <c r="B11" t="s" s="4">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="C11" s="10">
         <v>2</v>
@@ -19687,10 +19705,10 @@
         <v>0</v>
       </c>
       <c r="E12" t="s" s="4">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="F12" t="s" s="4">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="G12" s="33">
         <v>0</v>
@@ -19708,13 +19726,13 @@
         <v>0</v>
       </c>
       <c r="D13" t="s" s="4">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="E13" s="10">
         <v>0</v>
       </c>
       <c r="F13" t="s" s="4">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="G13" s="33">
         <v>0</v>
@@ -19735,7 +19753,7 @@
         <v>0</v>
       </c>
       <c r="E14" t="s" s="4">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="F14" s="10">
         <v>0</v>
@@ -19756,7 +19774,7 @@
         <v>0</v>
       </c>
       <c r="D15" t="s" s="4">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="E15" s="10">
         <v>0</v>
@@ -19774,7 +19792,7 @@
     <row r="16" ht="15" customHeight="1">
       <c r="A16" s="3"/>
       <c r="B16" t="s" s="4">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="C16" s="10">
         <v>0</v>
@@ -19804,10 +19822,10 @@
         <v>0</v>
       </c>
       <c r="D17" t="s" s="4">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="E17" t="s" s="4">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="F17" s="10">
         <v>0</v>
@@ -19834,7 +19852,7 @@
         <v>0</v>
       </c>
       <c r="F18" t="s" s="4">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="G18" s="33">
         <v>0</v>
@@ -19858,7 +19876,7 @@
         <v>0</v>
       </c>
       <c r="F19" t="s" s="4">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="G19" s="33">
         <v>1</v>
@@ -19870,7 +19888,7 @@
     <row r="20" ht="15" customHeight="1">
       <c r="A20" s="3"/>
       <c r="B20" t="s" s="4">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="C20" s="10">
         <v>1</v>
@@ -19894,16 +19912,16 @@
     <row r="21" ht="15" customHeight="1">
       <c r="A21" s="3"/>
       <c r="B21" t="s" s="4">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="C21" s="10">
         <v>1</v>
       </c>
       <c r="D21" t="s" s="4">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="E21" t="s" s="4">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="F21" s="10">
         <v>0</v>
@@ -19918,16 +19936,16 @@
     <row r="22" ht="15" customHeight="1">
       <c r="A22" s="3"/>
       <c r="B22" t="s" s="4">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="C22" s="10">
         <v>2</v>
       </c>
       <c r="D22" t="s" s="4">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="E22" t="s" s="4">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="F22" s="10">
         <v>0</v>
@@ -19962,7 +19980,7 @@
     <row r="25" ht="15" customHeight="1">
       <c r="A25" s="3"/>
       <c r="B25" t="s" s="6">
-        <v>425</v>
+        <v>431</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -19998,19 +20016,19 @@
       <c r="F27" s="35"/>
       <c r="G27" s="36"/>
       <c r="H27" t="s" s="37">
-        <v>423</v>
+        <v>429</v>
       </c>
     </row>
     <row r="28" ht="15" customHeight="1">
       <c r="A28" s="3"/>
       <c r="B28" t="s" s="20">
-        <v>426</v>
+        <v>432</v>
       </c>
       <c r="C28" t="s" s="20">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="D28" t="s" s="20">
-        <v>427</v>
+        <v>433</v>
       </c>
       <c r="E28" s="38"/>
       <c r="F28" s="38"/>
@@ -20022,13 +20040,13 @@
     <row r="29" ht="15" customHeight="1">
       <c r="A29" s="3"/>
       <c r="B29" t="s" s="4">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="C29" t="s" s="4">
-        <v>428</v>
+        <v>434</v>
       </c>
       <c r="D29" t="s" s="4">
-        <v>427</v>
+        <v>433</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
@@ -20040,13 +20058,13 @@
     <row r="30" ht="15" customHeight="1">
       <c r="A30" s="3"/>
       <c r="B30" t="s" s="4">
-        <v>426</v>
+        <v>432</v>
       </c>
       <c r="C30" t="s" s="4">
-        <v>428</v>
+        <v>434</v>
       </c>
       <c r="D30" t="s" s="4">
-        <v>424</v>
+        <v>430</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -20108,14 +20126,14 @@
     <row r="2" ht="15" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" t="s" s="6">
-        <v>429</v>
+        <v>435</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" t="s" s="6">
-        <v>430</v>
+        <v>436</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -20128,14 +20146,14 @@
     <row r="3" ht="15" customHeight="1">
       <c r="A3" s="3"/>
       <c r="B3" t="s" s="4">
-        <v>431</v>
+        <v>437</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" t="s" s="4">
-        <v>432</v>
+        <v>438</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -20155,7 +20173,7 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" t="s" s="43">
-        <v>433</v>
+        <v>439</v>
       </c>
       <c r="J4" s="35"/>
       <c r="K4" s="35"/>
@@ -20172,29 +20190,29 @@
         <v>18</v>
       </c>
       <c r="D5" t="s" s="17">
-        <v>434</v>
+        <v>440</v>
       </c>
       <c r="E5" t="s" s="17">
-        <v>435</v>
+        <v>441</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" t="s" s="44">
         <v>19</v>
       </c>
       <c r="H5" t="s" s="45">
-        <v>436</v>
+        <v>442</v>
       </c>
       <c r="I5" t="s" s="46">
-        <v>437</v>
+        <v>443</v>
       </c>
       <c r="J5" t="s" s="46">
-        <v>438</v>
+        <v>444</v>
       </c>
       <c r="K5" t="s" s="46">
-        <v>439</v>
+        <v>445</v>
       </c>
       <c r="L5" t="s" s="46">
-        <v>440</v>
+        <v>446</v>
       </c>
       <c r="M5" s="47"/>
       <c r="N5" s="47"/>
@@ -20208,10 +20226,10 @@
         <v>1</v>
       </c>
       <c r="D6" t="s" s="20">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="E6" t="s" s="20">
-        <v>442</v>
+        <v>448</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" t="s" s="48">
@@ -20248,7 +20266,7 @@
         <v>2</v>
       </c>
       <c r="D7" t="s" s="4">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="E7" s="10">
         <v>5</v>
@@ -20288,7 +20306,7 @@
         <v>3</v>
       </c>
       <c r="D8" t="s" s="4">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="E8" s="10">
         <v>6</v>
@@ -20328,32 +20346,32 @@
         <v>4</v>
       </c>
       <c r="D9" t="s" s="4">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="E9" t="s" s="4">
-        <v>442</v>
+        <v>448</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" t="s" s="49">
         <v>296</v>
       </c>
       <c r="H9" t="s" s="50">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="I9" s="10">
         <v>2</v>
       </c>
       <c r="J9" t="s" s="4">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="K9" t="s" s="4">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="L9" s="10">
         <v>2</v>
       </c>
       <c r="M9" t="s" s="4">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="N9" s="10">
         <v>2</v>
@@ -20368,7 +20386,7 @@
         <v>5</v>
       </c>
       <c r="D10" t="s" s="4">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="E10" s="10">
         <v>5</v>
@@ -20378,22 +20396,22 @@
         <v>297</v>
       </c>
       <c r="H10" t="s" s="50">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="I10" s="10">
         <v>2</v>
       </c>
       <c r="J10" t="s" s="4">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="K10" t="s" s="4">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="L10" s="10">
         <v>2</v>
       </c>
       <c r="M10" t="s" s="4">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="N10" s="10">
         <v>2</v>
@@ -20408,7 +20426,7 @@
         <v>6</v>
       </c>
       <c r="D11" t="s" s="4">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="E11" s="10">
         <v>6</v>
@@ -20448,26 +20466,26 @@
         <v>7</v>
       </c>
       <c r="D12" t="s" s="4">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="E12" t="s" s="4">
-        <v>442</v>
+        <v>448</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" t="s" s="49">
         <v>299</v>
       </c>
       <c r="H12" t="s" s="50">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="I12" t="s" s="4">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="J12" s="10">
         <v>2</v>
       </c>
       <c r="K12" t="s" s="4">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="L12" s="10">
         <v>3</v>
@@ -20488,7 +20506,7 @@
         <v>8</v>
       </c>
       <c r="D13" t="s" s="4">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="E13" s="10">
         <v>5</v>
@@ -20498,16 +20516,16 @@
         <v>300</v>
       </c>
       <c r="H13" t="s" s="50">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="I13" t="s" s="4">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="J13" s="10">
         <v>2</v>
       </c>
       <c r="K13" t="s" s="4">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="L13" s="10">
         <v>3</v>
@@ -20528,7 +20546,7 @@
         <v>9</v>
       </c>
       <c r="D14" t="s" s="4">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="E14" s="10">
         <v>6</v>
@@ -20568,7 +20586,7 @@
         <v>10</v>
       </c>
       <c r="D15" t="s" s="4">
-        <v>444</v>
+        <v>450</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
@@ -20606,29 +20624,29 @@
         <v>11</v>
       </c>
       <c r="D16" t="s" s="4">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="E16" t="s" s="4">
-        <v>442</v>
+        <v>448</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" t="s" s="49">
         <v>303</v>
       </c>
       <c r="H16" t="s" s="50">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="I16" t="s" s="4">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="J16" t="s" s="4">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="K16" s="10">
         <v>2</v>
       </c>
       <c r="L16" t="s" s="4">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="M16" s="10">
         <v>3</v>
@@ -20646,7 +20664,7 @@
         <v>12</v>
       </c>
       <c r="D17" t="s" s="4">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="E17" s="10">
         <v>5</v>
@@ -20656,19 +20674,19 @@
         <v>304</v>
       </c>
       <c r="H17" t="s" s="50">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="I17" t="s" s="4">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="J17" t="s" s="4">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="K17" s="10">
         <v>2</v>
       </c>
       <c r="L17" t="s" s="4">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="M17" s="10">
         <v>3</v>
@@ -20686,7 +20704,7 @@
         <v>13</v>
       </c>
       <c r="D18" t="s" s="4">
-        <v>441</v>
+        <v>447</v>
       </c>
       <c r="E18" s="10">
         <v>6</v>
@@ -20696,7 +20714,7 @@
         <v>305</v>
       </c>
       <c r="H18" t="s" s="50">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="I18" s="10">
         <v>2</v>
@@ -20741,7 +20759,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" t="s" s="4">
-        <v>445</v>
+        <v>451</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
@@ -20759,7 +20777,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" t="s" s="4">
-        <v>446</v>
+        <v>452</v>
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
@@ -20777,7 +20795,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" t="s" s="4">
-        <v>447</v>
+        <v>453</v>
       </c>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>

</xml_diff>